<commit_message>
First Commit to the Project
</commit_message>
<xml_diff>
--- a/testdata/TestData.xlsx
+++ b/testdata/TestData.xlsx
@@ -1,31 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23231"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vinesh.c\Downloads\Cucumber_SFDC-master\testdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vinesh.c\git\Cucumber_Maven_AutoRabit\Cucumber_SFDC-master\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{003920F5-3DD9-466F-BE6A-E12A14172807}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91F7D6A0-396B-4C99-836C-C3913C2DA28D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="3" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Login into salesforce page" sheetId="18" r:id="rId1"/>
     <sheet name="Account Creation and Verify" sheetId="19" r:id="rId2"/>
     <sheet name="Contact Creation and Verify" sheetId="20" r:id="rId3"/>
     <sheet name="Opportunity Creation and Verify" sheetId="15" r:id="rId4"/>
-    <sheet name="Publish the Wizard page changes" sheetId="16" r:id="rId5"/>
-    <sheet name="AHM Automation Use Case 2" sheetId="17" r:id="rId6"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="31">
   <si>
     <t>Scenario Name</t>
   </si>
@@ -45,84 +43,6 @@
     <t>password</t>
   </si>
   <si>
-    <t>passw0rd2</t>
-  </si>
-  <si>
-    <t>prudhvi@ahmopd1.dev</t>
-  </si>
-  <si>
-    <t>TC_03 Publish the Wizard page changes</t>
-  </si>
-  <si>
-    <t>Lightning App Builder</t>
-  </si>
-  <si>
-    <t>A_CSLT_Initiate_Wizard</t>
-  </si>
-  <si>
-    <t>ManageExpertCompensation</t>
-  </si>
-  <si>
-    <t>Expert</t>
-  </si>
-  <si>
-    <t>expert</t>
-  </si>
-  <si>
-    <t>A_CSLT-Initiate Wizard</t>
-  </si>
-  <si>
-    <t>UserFlowManagement</t>
-  </si>
-  <si>
-    <t>User Flow Management</t>
-  </si>
-  <si>
-    <t>Custom Metadata Types</t>
-  </si>
-  <si>
-    <t>Screen Configuration</t>
-  </si>
-  <si>
-    <t>ManageHCPExpert</t>
-  </si>
-  <si>
-    <t>Save</t>
-  </si>
-  <si>
-    <t>AHM Automation Use Case 2</t>
-  </si>
-  <si>
-    <t>rep.us-sg.a1r1d1t1@ahmopd1.dev</t>
-  </si>
-  <si>
-    <t>passw0rd1</t>
-  </si>
-  <si>
-    <t>Interaction test</t>
-  </si>
-  <si>
-    <t>Dec 31, 2018</t>
-  </si>
-  <si>
-    <t>Deepmala Rep</t>
-  </si>
-  <si>
-    <t>Nov 30, 2018</t>
-  </si>
-  <si>
-    <t>repdeepmala@ahmopd1.dev</t>
-  </si>
-  <si>
-    <t>passw0rd</t>
-  </si>
-  <si>
-    <t>username1</t>
-  </si>
-  <si>
-    <t>password1</t>
-  </si>
-  <si>
     <t>Login into salesforce application</t>
   </si>
   <si>
@@ -186,29 +106,23 @@
     <t>Create Opportunity and Verify</t>
   </si>
   <si>
-    <t>AutoRabit-QA@brillio.com</t>
-  </si>
-  <si>
-    <t>autorabit@2020</t>
-  </si>
-  <si>
     <t>appname</t>
   </si>
   <si>
     <t>Sales Console</t>
   </si>
   <si>
-    <t>autorabit@testing.com</t>
-  </si>
-  <si>
-    <t>Brillio@2020</t>
+    <t>rattankaur@circleci.qa</t>
+  </si>
+  <si>
+    <t>CircleCi.qa1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="22" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -351,18 +265,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="7"/>
-      <color rgb="FF222222"/>
-      <name val="Consolas"/>
-      <family val="3"/>
-    </font>
-    <font>
-      <sz val="7"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="9"/>
@@ -713,23 +615,17 @@
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="23" borderId="0" xfId="32"/>
     <xf numFmtId="49" fontId="1" fillId="23" borderId="0" xfId="32" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1113,7 +1009,7 @@
   <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="B2:E2"/>
+      <selection activeCell="B2" sqref="B2:E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1158,31 +1054,31 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>32</v>
+        <v>6</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="D2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="8" t="s">
-        <v>58</v>
+      <c r="E2" s="5" t="s">
+        <v>30</v>
       </c>
       <c r="F2" t="s">
-        <v>34</v>
+        <v>8</v>
       </c>
       <c r="G2" t="s">
-        <v>33</v>
+        <v>7</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>55</v>
+        <v>27</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>56</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -1192,8 +1088,8 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" xr:uid="{58388BCF-77FC-4BC6-97E4-8D411A2822F4}"/>
-    <hyperlink ref="E2" r:id="rId2" xr:uid="{BE30A098-3288-4EFB-BEE7-CDC6A1668DEF}"/>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{1F531DE0-EF55-4EEC-8AE9-ACBDCEA84B60}"/>
+    <hyperlink ref="E2" r:id="rId2" display="Brillio@2020" xr:uid="{4AB63531-C79E-4695-87BE-D4A9EFB41133}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId3"/>
@@ -1242,19 +1138,19 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>35</v>
+        <v>9</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>57</v>
+        <v>29</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="8" t="s">
-        <v>58</v>
+      <c r="E2" s="5" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -1264,8 +1160,8 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" xr:uid="{CE8ADFD4-B47E-4BA8-9977-105CBC740A23}"/>
-    <hyperlink ref="E2" r:id="rId2" xr:uid="{609AE5B7-0857-425D-9E7D-6A834BDB0467}"/>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{31DBB174-A31F-4E28-8CE4-B064BEE61270}"/>
+    <hyperlink ref="E2" r:id="rId2" display="Brillio@2020" xr:uid="{3BBA48C3-B057-4D0F-B979-1E840CEA55BD}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1275,8 +1171,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89006C19-397B-429E-860D-BBAA9A5FEF05}">
   <dimension ref="A1:O3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:E2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="B2:E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1342,37 +1238,37 @@
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>36</v>
+        <v>10</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>57</v>
+        <v>29</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="F2" s="9" t="s">
-        <v>37</v>
+      <c r="E2" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>11</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="H2" s="9" t="s">
-        <v>39</v>
+        <v>12</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>13</v>
       </c>
       <c r="I2" t="s">
-        <v>42</v>
-      </c>
-      <c r="J2" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="K2" s="10" t="s">
-        <v>41</v>
+        <v>16</v>
+      </c>
+      <c r="J2" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="K2" s="7" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
@@ -1389,7 +1285,7 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1" xr:uid="{B0C49C45-73D1-4D55-B57A-2E7C9B89C323}"/>
-    <hyperlink ref="E2" r:id="rId2" xr:uid="{22D2610A-CE9A-4ECB-8144-FF8B09801678}"/>
+    <hyperlink ref="E2" r:id="rId2" display="Brillio@2020" xr:uid="{22D2610A-CE9A-4ECB-8144-FF8B09801678}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId3"/>
@@ -1400,8 +1296,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:E2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1475,57 +1371,57 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>52</v>
+        <v>26</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="11" t="s">
-        <v>53</v>
+      <c r="C2" s="4" t="s">
+        <v>29</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="F2" s="9" t="s">
-        <v>43</v>
+      <c r="E2" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>17</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="H2" s="9" t="s">
-        <v>45</v>
+        <v>18</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>19</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="J2" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="K2" s="9" t="s">
-        <v>48</v>
+        <v>20</v>
+      </c>
+      <c r="J2" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="K2" s="6" t="s">
+        <v>22</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>49</v>
+        <v>23</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>50</v>
+        <v>24</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>39</v>
+        <v>13</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>42</v>
+        <v>16</v>
       </c>
       <c r="P2" s="1" t="s">
-        <v>51</v>
+        <v>25</v>
       </c>
       <c r="Q2" s="1" t="s">
-        <v>41</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
@@ -1535,394 +1431,10 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" xr:uid="{7A2D7D8C-8D86-40F8-A65F-C120051230CC}"/>
-    <hyperlink ref="E2" r:id="rId2" xr:uid="{106152D0-BEF9-4A20-8448-63D8937043E2}"/>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{53D3F7CB-4658-4D2B-8376-2E9538F11762}"/>
+    <hyperlink ref="E2" r:id="rId2" display="Brillio@2020" xr:uid="{7211713E-D7B0-41B1-AB52-504C347892D2}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:AI3"/>
-  <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="33.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="20.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="13" width="24.85546875" bestFit="1" customWidth="1"/>
-    <col min="17" max="18" width="19.7109375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="N1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="O1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="P1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="Q1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="R1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="S1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="T1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="U1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="V1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="W1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="X1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="Y1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="Z1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="AA1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="AB1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="AC1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="AD1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="AE1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="AF1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="AG1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="AH1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="AI1" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G2" t="s">
-        <v>9</v>
-      </c>
-      <c r="H2" t="s">
-        <v>10</v>
-      </c>
-      <c r="I2" t="s">
-        <v>10</v>
-      </c>
-      <c r="J2" t="s">
-        <v>10</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="M2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="N2" t="s">
-        <v>12</v>
-      </c>
-      <c r="O2" t="s">
-        <v>13</v>
-      </c>
-      <c r="P2" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q2" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="R2" t="s">
-        <v>14</v>
-      </c>
-      <c r="S2" t="s">
-        <v>14</v>
-      </c>
-      <c r="T2" t="s">
-        <v>17</v>
-      </c>
-      <c r="U2" t="s">
-        <v>17</v>
-      </c>
-      <c r="V2" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="W2" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="X2" t="s">
-        <v>18</v>
-      </c>
-      <c r="Y2" t="s">
-        <v>18</v>
-      </c>
-      <c r="Z2" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="AA2" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="AB2" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="AC2" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="AD2" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="AE2" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="AF2" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="AG2" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="AH2" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="AI2" s="6" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="3" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:Q3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:A3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="24.7109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="20.85546875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="N1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="O1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="P1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="Q1" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="D2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E2" t="s">
-        <v>23</v>
-      </c>
-      <c r="F2" t="s">
-        <v>24</v>
-      </c>
-      <c r="G2" t="s">
-        <v>24</v>
-      </c>
-      <c r="H2" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="I2" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="J2" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="K2" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="L2" t="s">
-        <v>26</v>
-      </c>
-      <c r="M2" t="s">
-        <v>26</v>
-      </c>
-      <c r="N2" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="O2" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="P2" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="1"/>
-      <c r="C3" s="4"/>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
-    <hyperlink ref="O2" r:id="rId2" xr:uid="{00000000-0004-0000-0200-000001000000}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>